<commit_message>
Neue Form für die Karten!!!
- mit Großbildfunktion ;)
</commit_message>
<xml_diff>
--- a/Prgramm/OrtsKoordinaten/Orte-Liste.xlsx
+++ b/Prgramm/OrtsKoordinaten/Orte-Liste.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="83">
   <si>
     <t>Berlin</t>
   </si>
@@ -259,15 +259,6 @@
   </si>
   <si>
     <t>KoSy-y</t>
-  </si>
-  <si>
-    <t>Lüneburg</t>
-  </si>
-  <si>
-    <t>Wismar</t>
-  </si>
-  <si>
-    <t>Schwerin</t>
   </si>
   <si>
     <t>Geesthacht</t>
@@ -661,8 +652,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E106"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" topLeftCell="A24" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -676,7 +667,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B1" s="9"/>
       <c r="C1" s="9"/>
@@ -1855,16 +1846,18 @@
         <v>81</v>
       </c>
       <c r="C81" s="4"/>
-      <c r="D81" s="2"/>
-      <c r="E81" s="2"/>
+      <c r="D81" s="2">
+        <v>950</v>
+      </c>
+      <c r="E81" s="2">
+        <v>566</v>
+      </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" s="2">
         <v>78</v>
       </c>
-      <c r="B82" s="2" t="s">
-        <v>82</v>
-      </c>
+      <c r="B82" s="2"/>
       <c r="C82" s="4"/>
       <c r="D82" s="2"/>
       <c r="E82" s="2"/>
@@ -1873,9 +1866,7 @@
       <c r="A83" s="2">
         <v>79</v>
       </c>
-      <c r="B83" s="2" t="s">
-        <v>83</v>
-      </c>
+      <c r="B83" s="2"/>
       <c r="C83" s="4"/>
       <c r="D83" s="2"/>
       <c r="E83" s="2"/>
@@ -1884,12 +1875,6 @@
       <c r="A84" s="2">
         <v>80</v>
       </c>
-      <c r="B84" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="C84" s="4"/>
-      <c r="D84" s="2"/>
-      <c r="E84" s="2"/>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" s="2">

</xml_diff>